<commit_message>
thinking about time consistency
</commit_message>
<xml_diff>
--- a/literature/record_estimating_learning.xlsx
+++ b/literature/record_estimating_learning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26020" yWindow="640" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Paper / book</t>
   </si>
@@ -39,9 +39,6 @@
     <t>CEMP</t>
   </si>
   <si>
-    <t>marginalized particle filter</t>
-  </si>
-  <si>
     <t>Milani 2007</t>
   </si>
   <si>
@@ -54,18 +51,12 @@
     <t>Milani 2014</t>
   </si>
   <si>
-    <t>Bayesian, endogenous gain</t>
-  </si>
-  <si>
     <t>Gust Herbst Lopez-Salido 2019</t>
   </si>
   <si>
     <t>Bayesian, constant gain</t>
   </si>
   <si>
-    <t>Bayesian, constant gain I think</t>
-  </si>
-  <si>
     <t>Branch Evans 2006 (says 2005 on the actualy pdf)</t>
   </si>
   <si>
@@ -76,6 +67,21 @@
   </si>
   <si>
     <t>avg w/o Malmendier or Gust et al.</t>
+  </si>
+  <si>
+    <t>marginalized particle filter: anchoring can match long-term inflation forecasts w/o targeting them (can explain Missing Deflation/Inflation)</t>
+  </si>
+  <si>
+    <t>Bayesian, constant gain I think: can match intertia in inflation</t>
+  </si>
+  <si>
+    <t>Bayesian, endogenous gain, model matches time-varying volatility of macro variables, high in Great Inflation, falling in Great Moderation</t>
+  </si>
+  <si>
+    <t>Eusepi Preston 2011 AER</t>
+  </si>
+  <si>
+    <t>outlier b/c calibrated, but their whole point is the quantitative performance is better than RE version, e.g. persistence and hum-shaped IRFs despite iid shocks.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -530,7 +536,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
         <v>0.14499999999999999</v>
@@ -541,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>0.05</v>
@@ -549,10 +555,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>1.83E-2</v>
@@ -560,10 +566,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>8.2000000000000003E-2</v>
@@ -571,10 +577,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <v>6.2E-2</v>
@@ -582,10 +588,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>3.044</v>
@@ -593,13 +599,21 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
         <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="3:4">
@@ -608,7 +622,7 @@
         <v>7.1459999999999996E-2</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>